<commit_message>
Added word lists generator | Fixed words, rt calc, screens according to code tests
Fixed PAS rt calc
aligned words with fixation cross
Improved word list
Added passed_tests file
Changed instructions screen
</commit_message>
<xml_diff>
--- a/development/passed_tests.xlsx
+++ b/development/passed_tests.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B91793-44D4-4FE6-813C-0244B156460C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
   <si>
     <t>Conditions:</t>
   </si>
@@ -79,9 +80,6 @@
     <t>Checklist</t>
   </si>
   <si>
-    <t>Sub list</t>
-  </si>
-  <si>
     <t>Masks visual angle is 2.5 X 1 deg</t>
   </si>
   <si>
@@ -368,12 +366,6 @@
   </si>
   <si>
     <t>optional, can check visualy</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Stimuli duration is correct</t>
@@ -399,13 +391,77 @@
   </si>
   <si>
     <t>mask=target=prime = 1mm</t>
+  </si>
+  <si>
+    <t>in 10 trials make sure there are: 
+mask1, mask2, prime, mask3, target, categor, recog,  pas</t>
+  </si>
+  <si>
+    <t>All words are imageable</t>
+  </si>
+  <si>
+    <t>Words don't repeat in stimuli list</t>
+  </si>
+  <si>
+    <t>make sure both conditions exist:
+artificial / natural
+same / diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mask1 = 270ms
+mask2 = 30ms
+prime = 30ms
+mask3 = 30ms
+target = 500ms
+</t>
+  </si>
+  <si>
+    <t>in 10 trials make sure masks cover prime and target</t>
+  </si>
+  <si>
+    <t>10 sec</t>
+  </si>
+  <si>
+    <t>10 trials have:
+categorization
+recognition
+pas</t>
+  </si>
+  <si>
+    <t>Elabration</t>
+  </si>
+  <si>
+    <t>run sub 123123 and sub 123122 and check</t>
+  </si>
+  <si>
+    <t>Fixation overlaps with stimuli and mask</t>
+  </si>
+  <si>
+    <t>240 so:
+artificial + same = 120
+artificial + diff = 120
+natural + same = 120
+natural + diff = 120
+A word repeats as target only twice in each block</t>
+  </si>
+  <si>
+    <t>10 No response on categor and recog: make sure you get PAS</t>
+  </si>
+  <si>
+    <t>1 response all: make sure the it is recorded after 10 last werent</t>
+  </si>
+  <si>
+    <t>11 No response on categor: make sure you get recog traj and PAS</t>
+  </si>
+  <si>
+    <t>9 No response on recog: make sure you get categor traj and PAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,8 +490,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,13 +520,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -478,12 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -492,10 +556,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,6 +589,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFCCFFFF"/>
     </mruColors>
   </colors>
@@ -594,6 +680,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -629,6 +732,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -804,18 +924,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="49.25" style="5" customWidth="1"/>
     <col min="4" max="4" width="27.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -824,7 +944,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>10</v>
@@ -834,18 +954,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
@@ -854,643 +976,751 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="19" t="s">
+        <v>125</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="22" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B13" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>125</v>
+      <c r="B15" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>26</v>
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>27</v>
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>12</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>12</v>
+      <c r="A18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>18</v>
+      <c r="B25" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>19</v>
+      <c r="A26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="4" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="D41" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D42" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="B53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="D53" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="D54" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="D55" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+      <c r="D56" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="B57" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="D57" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="D58" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="9"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="9"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="9"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="9"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="9"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="9"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B107" s="9"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="9"/>
+      <c r="A108" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B110" s="10"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
+      <c r="A110" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B113" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
+      <c r="B112" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>